<commit_message>
more gemini and bing search results
</commit_message>
<xml_diff>
--- a/LLMWithWebData/GeminiWithSearchGrounding/GeminiWithGroundingVersionNotes.xlsx
+++ b/LLMWithWebData/GeminiWithSearchGrounding/GeminiWithGroundingVersionNotes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/feyzjan/GithubRepos/EquifaxPracticum/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/feyzjan/GithubRepos/EquifaxPracticum/LLMWithWebData/GeminiWithSearchGrounding/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{31FBFA9E-B19D-D34B-9741-4350895E0260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E031B8-3394-D348-9AFD-D6C4302624AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17200" xr2:uid="{2CC064C5-46D9-9C4F-9719-C33FB8014C2D}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>Version</t>
   </si>
@@ -115,6 +115,21 @@
   </si>
   <si>
     <t>firm_properties_gemini_with_grounding_v1</t>
+  </si>
+  <si>
+    <t>v2</t>
+  </si>
+  <si>
+    <t>Changes</t>
+  </si>
+  <si>
+    <t>Added new fields</t>
+  </si>
+  <si>
+    <t>Firm</t>
+  </si>
+  <si>
+    <t>Complete?</t>
   </si>
 </sst>
 </file>
@@ -210,15 +225,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D733AC42-A8C0-CB46-97CF-98099047A0E0}" name="Table134" displayName="Table134" ref="A1:F2" totalsRowShown="0">
-  <autoFilter ref="A1:F2" xr:uid="{D733AC42-A8C0-CB46-97CF-98099047A0E0}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D733AC42-A8C0-CB46-97CF-98099047A0E0}" name="Table134" displayName="Table134" ref="A1:H3" totalsRowShown="0">
+  <autoFilter ref="A1:H3" xr:uid="{D733AC42-A8C0-CB46-97CF-98099047A0E0}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{A453A5C3-533D-2845-9F3E-FAAB3E838C0A}" name="Version"/>
+    <tableColumn id="7" xr3:uid="{0A52686F-647E-1E49-B284-C74308E5D6E9}" name="Changes"/>
     <tableColumn id="4" xr3:uid="{EFF0BE4F-9E56-9D4C-ADA4-51DD394E1B57}" name="Model"/>
-    <tableColumn id="2" xr3:uid="{FF99AE5B-8771-5844-9836-D2299DB47D60}" name="Used Prompts" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{F5DB8BCC-64FC-7F4D-8F7A-402D81605DE3}" name="Query for every" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{FF99AE5B-8771-5844-9836-D2299DB47D60}" name="Used Prompts" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{F5DB8BCC-64FC-7F4D-8F7A-402D81605DE3}" name="Query for every" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{4E643F53-1076-5E4B-A502-99C4872A4D16}" name="Note"/>
     <tableColumn id="5" xr3:uid="{9E0414FC-0BEE-3F48-86C0-43FF58E80C37}" name="Google Search"/>
+    <tableColumn id="8" xr3:uid="{CA8020E4-E959-2B46-BF3E-9D6022C3CD50}" name="Complete?"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -229,7 +246,7 @@
   <autoFilter ref="A1:C2" xr:uid="{670D22A1-F5E2-3E45-AA94-FAC9DB9C9ACE}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{EE71C30A-2B49-234D-96BE-1F1147285179}" name="Version"/>
-    <tableColumn id="2" xr3:uid="{04AE3823-4358-934A-B029-EF2D7A86C32E}" name="Content" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{04AE3823-4358-934A-B029-EF2D7A86C32E}" name="Content" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{A9AE875C-182C-2A44-9441-34589AB24AA1}" name="Note"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -241,7 +258,7 @@
   <autoFilter ref="A1:C2" xr:uid="{7A2CC917-32D2-034B-B934-C2D8689008FE}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{836ADFF3-065B-5C4A-A416-5AAB7C3480E0}" name="Version"/>
-    <tableColumn id="2" xr3:uid="{83ED2170-E5EB-7145-8C07-65CDEB6031E3}" name="Content" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{83ED2170-E5EB-7145-8C07-65CDEB6031E3}" name="Content" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{30D926A8-6225-3346-AB03-B379976B68D7}" name="Note"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -253,7 +270,7 @@
   <autoFilter ref="A1:C8" xr:uid="{5B97AC83-C3A6-064D-9231-23EB55BF9A9C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8412D800-6229-1848-BBDE-3760933C0DBA}" name="Version"/>
-    <tableColumn id="2" xr3:uid="{BC1A659E-1728-6643-BBD1-7D0740C6C4E3}" name="Used Prompts" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{BC1A659E-1728-6643-BBD1-7D0740C6C4E3}" name="Used Prompts" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{390C8958-367F-914A-9B52-0BA71EFD7EFD}" name="Note"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -577,55 +594,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{947C3434-E968-E844-A53E-A02EE656E774}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" customWidth="1"/>
-    <col min="3" max="3" width="68.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="68.83203125" customWidth="1"/>
+    <col min="2" max="2" width="36" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" customWidth="1"/>
+    <col min="4" max="4" width="68.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish gemini with grounding
</commit_message>
<xml_diff>
--- a/LLMWithWebData/GeminiWithSearchGrounding/GeminiWithGroundingVersionNotes.xlsx
+++ b/LLMWithWebData/GeminiWithSearchGrounding/GeminiWithGroundingVersionNotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/feyzjan/GithubRepos/EquifaxPracticum/LLMWithWebData/GeminiWithSearchGrounding/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E031B8-3394-D348-9AFD-D6C4302624AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3063398-D304-584A-9AB0-EC734E9057A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17200" xr2:uid="{2CC064C5-46D9-9C4F-9719-C33FB8014C2D}"/>
+    <workbookView xWindow="1100" yWindow="760" windowWidth="28040" windowHeight="17140" xr2:uid="{2CC064C5-46D9-9C4F-9719-C33FB8014C2D}"/>
   </bookViews>
   <sheets>
     <sheet name="VersionNotes" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
   <si>
     <t>Version</t>
   </si>
@@ -111,15 +111,9 @@
     <t>Field</t>
   </si>
   <si>
-    <t>answer_format_1, field_to_query_1</t>
-  </si>
-  <si>
     <t>firm_properties_gemini_with_grounding_v1</t>
   </si>
   <si>
-    <t>v2</t>
-  </si>
-  <si>
     <t>Changes</t>
   </si>
   <si>
@@ -130,6 +124,33 @@
   </si>
   <si>
     <t>Complete?</t>
+  </si>
+  <si>
+    <t>firm_properties_gemini_with_grounding_v2</t>
+  </si>
+  <si>
+    <t>firm_properties_gemini_without_grounding_local_dataset_v1</t>
+  </si>
+  <si>
+    <t>context</t>
+  </si>
+  <si>
+    <t>context_single_answer_v1 + context_local_dataset_v1</t>
+  </si>
+  <si>
+    <t>context_single_answer_v1</t>
+  </si>
+  <si>
+    <t>Answer Format</t>
+  </si>
+  <si>
+    <t>Field prompts</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> field_to_query_1</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -195,7 +216,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -225,14 +249,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D733AC42-A8C0-CB46-97CF-98099047A0E0}" name="Table134" displayName="Table134" ref="A1:H3" totalsRowShown="0">
-  <autoFilter ref="A1:H3" xr:uid="{D733AC42-A8C0-CB46-97CF-98099047A0E0}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D733AC42-A8C0-CB46-97CF-98099047A0E0}" name="Table134" displayName="Table134" ref="A1:J4" totalsRowShown="0">
+  <autoFilter ref="A1:J4" xr:uid="{D733AC42-A8C0-CB46-97CF-98099047A0E0}"/>
+  <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{A453A5C3-533D-2845-9F3E-FAAB3E838C0A}" name="Version"/>
     <tableColumn id="7" xr3:uid="{0A52686F-647E-1E49-B284-C74308E5D6E9}" name="Changes"/>
     <tableColumn id="4" xr3:uid="{EFF0BE4F-9E56-9D4C-ADA4-51DD394E1B57}" name="Model"/>
-    <tableColumn id="2" xr3:uid="{FF99AE5B-8771-5844-9836-D2299DB47D60}" name="Used Prompts" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{F5DB8BCC-64FC-7F4D-8F7A-402D81605DE3}" name="Query for every" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{8E6E8868-F72D-5540-954F-5D125D4AF3D2}" name="context"/>
+    <tableColumn id="2" xr3:uid="{FF99AE5B-8771-5844-9836-D2299DB47D60}" name="Answer Format" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{C3036B1B-F3ED-0D4F-A1B7-B321910E1974}" name="Field prompts" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{F5DB8BCC-64FC-7F4D-8F7A-402D81605DE3}" name="Query for every" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{4E643F53-1076-5E4B-A502-99C4872A4D16}" name="Note"/>
     <tableColumn id="5" xr3:uid="{9E0414FC-0BEE-3F48-86C0-43FF58E80C37}" name="Google Search"/>
     <tableColumn id="8" xr3:uid="{CA8020E4-E959-2B46-BF3E-9D6022C3CD50}" name="Complete?"/>
@@ -246,7 +272,7 @@
   <autoFilter ref="A1:C2" xr:uid="{670D22A1-F5E2-3E45-AA94-FAC9DB9C9ACE}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{EE71C30A-2B49-234D-96BE-1F1147285179}" name="Version"/>
-    <tableColumn id="2" xr3:uid="{04AE3823-4358-934A-B029-EF2D7A86C32E}" name="Content" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{04AE3823-4358-934A-B029-EF2D7A86C32E}" name="Content" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{A9AE875C-182C-2A44-9441-34589AB24AA1}" name="Note"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -258,7 +284,7 @@
   <autoFilter ref="A1:C2" xr:uid="{7A2CC917-32D2-034B-B934-C2D8689008FE}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{836ADFF3-065B-5C4A-A416-5AAB7C3480E0}" name="Version"/>
-    <tableColumn id="2" xr3:uid="{83ED2170-E5EB-7145-8C07-65CDEB6031E3}" name="Content" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{83ED2170-E5EB-7145-8C07-65CDEB6031E3}" name="Content" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{30D926A8-6225-3346-AB03-B379976B68D7}" name="Note"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -270,7 +296,7 @@
   <autoFilter ref="A1:C8" xr:uid="{5B97AC83-C3A6-064D-9231-23EB55BF9A9C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8412D800-6229-1848-BBDE-3760933C0DBA}" name="Version"/>
-    <tableColumn id="2" xr3:uid="{BC1A659E-1728-6643-BBD1-7D0740C6C4E3}" name="Used Prompts" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{BC1A659E-1728-6643-BBD1-7D0740C6C4E3}" name="Used Prompts" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{390C8958-367F-914A-9B52-0BA71EFD7EFD}" name="Note"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -594,89 +620,123 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{947C3434-E968-E844-A53E-A02EE656E774}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" customWidth="1"/>
-    <col min="4" max="4" width="68.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="68.83203125" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="68.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
         <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="J1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="E2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="J2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
         <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>17</v>
+      <c r="D3" t="s">
+        <v>26</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
         <v>14</v>
       </c>
-      <c r="H3">
-        <v>1000</v>
+      <c r="J3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="J4" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>

<commit_message>
finished generating two results datasets
</commit_message>
<xml_diff>
--- a/LLMWithWebData/GeminiWithSearchGrounding/GeminiWithGroundingVersionNotes.xlsx
+++ b/LLMWithWebData/GeminiWithSearchGrounding/GeminiWithGroundingVersionNotes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/feyzjan/GithubRepos/EquifaxPracticum/LLMWithWebData/GeminiWithSearchGrounding/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3063398-D304-584A-9AB0-EC734E9057A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8769B39B-6796-A641-812D-BF91765841C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="760" windowWidth="28040" windowHeight="17140" xr2:uid="{2CC064C5-46D9-9C4F-9719-C33FB8014C2D}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>Version</t>
   </si>
@@ -108,12 +108,6 @@
     <t>Query for every</t>
   </si>
   <si>
-    <t>Field</t>
-  </si>
-  <si>
-    <t>firm_properties_gemini_with_grounding_v1</t>
-  </si>
-  <si>
     <t>Changes</t>
   </si>
   <si>
@@ -150,7 +144,7 @@
     <t xml:space="preserve"> field_to_query_1</t>
   </si>
   <si>
-    <t>-</t>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -249,16 +243,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D733AC42-A8C0-CB46-97CF-98099047A0E0}" name="Table134" displayName="Table134" ref="A1:J4" totalsRowShown="0">
-  <autoFilter ref="A1:J4" xr:uid="{D733AC42-A8C0-CB46-97CF-98099047A0E0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D733AC42-A8C0-CB46-97CF-98099047A0E0}" name="Table134" displayName="Table134" ref="A1:J3" totalsRowShown="0">
+  <autoFilter ref="A1:J3" xr:uid="{D733AC42-A8C0-CB46-97CF-98099047A0E0}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{A453A5C3-533D-2845-9F3E-FAAB3E838C0A}" name="Version"/>
     <tableColumn id="7" xr3:uid="{0A52686F-647E-1E49-B284-C74308E5D6E9}" name="Changes"/>
     <tableColumn id="4" xr3:uid="{EFF0BE4F-9E56-9D4C-ADA4-51DD394E1B57}" name="Model"/>
     <tableColumn id="10" xr3:uid="{8E6E8868-F72D-5540-954F-5D125D4AF3D2}" name="context"/>
     <tableColumn id="2" xr3:uid="{FF99AE5B-8771-5844-9836-D2299DB47D60}" name="Answer Format" dataDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{C3036B1B-F3ED-0D4F-A1B7-B321910E1974}" name="Field prompts" dataDxfId="0"/>
-    <tableColumn id="6" xr3:uid="{F5DB8BCC-64FC-7F4D-8F7A-402D81605DE3}" name="Query for every" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{C3036B1B-F3ED-0D4F-A1B7-B321910E1974}" name="Field prompts" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{F5DB8BCC-64FC-7F4D-8F7A-402D81605DE3}" name="Query for every" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{4E643F53-1076-5E4B-A502-99C4872A4D16}" name="Note"/>
     <tableColumn id="5" xr3:uid="{9E0414FC-0BEE-3F48-86C0-43FF58E80C37}" name="Google Search"/>
     <tableColumn id="8" xr3:uid="{CA8020E4-E959-2B46-BF3E-9D6022C3CD50}" name="Complete?"/>
@@ -272,7 +266,7 @@
   <autoFilter ref="A1:C2" xr:uid="{670D22A1-F5E2-3E45-AA94-FAC9DB9C9ACE}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{EE71C30A-2B49-234D-96BE-1F1147285179}" name="Version"/>
-    <tableColumn id="2" xr3:uid="{04AE3823-4358-934A-B029-EF2D7A86C32E}" name="Content" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{04AE3823-4358-934A-B029-EF2D7A86C32E}" name="Content" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{A9AE875C-182C-2A44-9441-34589AB24AA1}" name="Note"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -284,7 +278,7 @@
   <autoFilter ref="A1:C2" xr:uid="{7A2CC917-32D2-034B-B934-C2D8689008FE}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{836ADFF3-065B-5C4A-A416-5AAB7C3480E0}" name="Version"/>
-    <tableColumn id="2" xr3:uid="{83ED2170-E5EB-7145-8C07-65CDEB6031E3}" name="Content" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{83ED2170-E5EB-7145-8C07-65CDEB6031E3}" name="Content" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{30D926A8-6225-3346-AB03-B379976B68D7}" name="Note"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -296,7 +290,7 @@
   <autoFilter ref="A1:C8" xr:uid="{5B97AC83-C3A6-064D-9231-23EB55BF9A9C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8412D800-6229-1848-BBDE-3760933C0DBA}" name="Version"/>
-    <tableColumn id="2" xr3:uid="{BC1A659E-1728-6643-BBD1-7D0740C6C4E3}" name="Used Prompts" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{BC1A659E-1728-6643-BBD1-7D0740C6C4E3}" name="Used Prompts" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{390C8958-367F-914A-9B52-0BA71EFD7EFD}" name="Note"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -620,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{947C3434-E968-E844-A53E-A02EE656E774}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -641,19 +635,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
         <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G1" t="s">
         <v>15</v>
@@ -665,73 +659,53 @@
         <v>13</v>
       </c>
       <c r="J1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
         <v>17</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
       </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
       <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="I2" t="s">
         <v>14</v>
       </c>
       <c r="J2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>20</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
       <c r="I3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" t="s">
         <v>14</v>
-      </c>
-      <c r="J3">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="J4" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>